<commit_message>
Fix bug on import date_of_birth
</commit_message>
<xml_diff>
--- a/subscriptions/core/tests/files/test.xlsx
+++ b/subscriptions/core/tests/files/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t xml:space="preserve">*Nome Completo</t>
   </si>
@@ -61,9 +61,6 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">12/08/1996</t>
-  </si>
-  <si>
     <t xml:space="preserve">Porto Alegre</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t xml:space="preserve">Lucas 2</t>
   </si>
   <si>
-    <t xml:space="preserve">13/08/1996</t>
-  </si>
-  <si>
     <t xml:space="preserve">2km</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t xml:space="preserve">Lucas 3</t>
   </si>
   <si>
-    <t xml:space="preserve">14/08/1996</t>
-  </si>
-  <si>
     <t xml:space="preserve">3km</t>
   </si>
   <si>
@@ -112,9 +103,6 @@
     <t xml:space="preserve">Lucas 4</t>
   </si>
   <si>
-    <t xml:space="preserve">15/08/1996</t>
-  </si>
-  <si>
     <t xml:space="preserve">4km</t>
   </si>
   <si>
@@ -125,9 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lucas 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16/08/1996</t>
   </si>
   <si>
     <t xml:space="preserve">5km</t>
@@ -142,13 +127,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -237,23 +223,23 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.53571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.18367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.42857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,23 +287,23 @@
       <c r="D2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1" t="n">
+        <v>35289</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,28 +311,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>35290</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>12</v>
@@ -357,31 +343,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>35291</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -389,31 +375,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>35292</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,28 +407,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
+      <c r="E6" s="1" t="n">
+        <v>35293</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="J6" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add subscription field paid
</commit_message>
<xml_diff>
--- a/subscriptions/core/tests/files/test.xlsx
+++ b/subscriptions/core/tests/files/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t xml:space="preserve">*Nome Completo</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">Tamanho da Camiseta</t>
   </si>
   <si>
+    <t xml:space="preserve">Pago</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lucas Rangel Cezimbra 1</t>
   </si>
   <si>
@@ -74,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Baby Look M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pendente</t>
   </si>
   <si>
     <t xml:space="preserve">Lucas Rangel Cezimbra 2</t>
@@ -220,26 +226,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L:L"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.42857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -273,37 +278,43 @@
       <c r="K1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>35289</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,31 +322,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>35290</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,31 +357,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>35291</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,31 +392,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>35292</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,28 +427,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>35293</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>